<commit_message>
Update acceptance test plan spreadsheet
Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -72,6 +72,9 @@
     <t xml:space="preserve">SJD; 2/28/18</t>
   </si>
   <si>
+    <t xml:space="preserve">MTD; 3/27/18</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that I am not signed-in when I do click on the sign-in link then I expect to be taken to the Signin page, with a means to enter a player name.</t>
   </si>
   <si>
@@ -108,7 +111,7 @@
     <t xml:space="preserve">Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View from the Home page.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given a valid, initial game board when I drag a piece to a white space then the piece should not be droppable.</t>
+    <t xml:space="preserve">Given a valid, initial game board when I drag a red piece to a white space then the piece should not be droppable.</t>
   </si>
   <si>
     <t xml:space="preserve">Given a valid, initial game board when I drag a piece to an occupied space then the piece should not be droppable.</t>
@@ -120,37 +123,94 @@
     <t xml:space="preserve">Given a valid, initial game board when I view the board in the browser then my pieces are oriented on the bottom of the board grid just like I would see the board if I were playing in the physical world.</t>
   </si>
   <si>
-    <t xml:space="preserve">Player Registration</t>
-  </si>
-  <si>
     <t xml:space="preserve">Player Sign-out</t>
   </si>
   <si>
-    <t xml:space="preserve">Game Requests</t>
+    <t xml:space="preserve">Given that I am currently signed in when I see the Home page then I must see a means to sign out.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am signed in when I click on the sign out button then I expect to be signed out and taken back to the Home page.</t>
   </si>
   <si>
     <t xml:space="preserve">Matchmaking</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am on the home page when I look at a player who is not in a game then I see some indicator showing that they are not in a game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am on the home page when I look at a player who is in a game then I see some indicator showing that they are in a game (so I can't challenge them).</t>
+  </si>
+  <si>
     <t xml:space="preserve">Player Turns</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am a Player in a game when I make a move then it would be the opposing Player's turn</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valid Moves</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am in a game and it's my turn, when I make a valid move then the move should complete without any errors or warning messages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am in a game and it's my turn, when I make an invalid move, then the move should not complete and I should see an error saying I tried to make an invalid move.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTD; 3/27/18; Moving a piece to a valid location, then moving it to any other location, causes a NullPointerException.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jumps</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when there is an opponents piece I can capture then I am able to make a single jump move and take that piece off the board and advance my piece.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when there are 2 or more opponents pieces that I can capture then I am able to make a multiple jump move and move those pieces off the board and advance my piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when I have multiple jumps that I can take then I am able to choose which jump I can make</t>
+  </si>
+  <si>
     <t xml:space="preserve">Forced Moves</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am a Player in a game when it is my turn and a jump move is possible then I have to make the full jump move in order to advance the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when it is my turn and a multiple jump move is possible then I must complete the entirety of the multiple jump move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am in a game, when it is my turn and more than one jump moves are possible, then I am forced to choose one of them to fully jump through.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Game Over</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am a Player in a game when I win/lose the game then I expect to redirected back to the Home Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when it is my turn and I am unable to  make a move then I will lose the game and be redirected to the Home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when all my pieces have been eliminated from the board then I will lose the game and be redirected to the Homepage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game, when my opponent loses the game, then I will win the game and be redirected to the home page.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Forfeiting</t>
   </si>
   <si>
-    <t xml:space="preserve">Forfeit Navigation</t>
+    <t xml:space="preserve">Given that I am a Player when I am in a game then I expect to be able to forfeit the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when I quit the application then I expect to forfeit the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player when I forfeit a game then I expect to be redirected to the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game, when my opponent forfeits the game then I will win the game and be redirected to the home page.</t>
   </si>
   <si>
     <t xml:space="preserve">King Creation</t>
@@ -500,12 +560,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C12" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="topRight" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -547,7 +607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -559,112 +619,138 @@
         <v>14</v>
       </c>
       <c r="E2" s="8"/>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="8"/>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="8"/>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="8"/>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="8"/>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="8"/>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="47.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="8"/>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="8"/>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="3" t="s">
@@ -673,213 +759,357 @@
       <c r="E11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="93.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="73.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="8"/>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="8"/>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="8"/>
+      <c r="F14" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="8"/>
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="8"/>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="11"/>
+    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="E17" s="8"/>
+      <c r="F17" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
+      <c r="AMJ17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="8"/>
       <c r="E18" s="8"/>
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="8"/>
       <c r="E19" s="8"/>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>34</v>
+    <row r="20" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="8"/>
       <c r="E20" s="8"/>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="8"/>
       <c r="E21" s="8"/>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="8"/>
       <c r="E22" s="8"/>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
+    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C23" s="8"/>
       <c r="E23" s="8"/>
+      <c r="F23" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C24" s="8"/>
       <c r="E24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>39</v>
+    <row r="25" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>40</v>
+    <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C26" s="8"/>
       <c r="E26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C27" s="8"/>
       <c r="E27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>42</v>
+    <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C28" s="8"/>
       <c r="E28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>43</v>
+    <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C29" s="8"/>
       <c r="E29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C30" s="8"/>
       <c r="E30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>45</v>
+    <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
-        <v>46</v>
+    <row r="32" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
-        <v>47</v>
+    <row r="33" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C33" s="8"/>
       <c r="E33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C34" s="8"/>
       <c r="E34" s="8"/>
       <c r="G34" s="8"/>
     </row>
+    <row r="35" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C597 E2:E597 G2:G597">
+  <conditionalFormatting sqref="C38:C607 E38:E607 G2:G607 C2:C37 E2:E37">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Pass"</formula>
     </cfRule>
@@ -887,7 +1117,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F597 H2:H597 D2:D597">
+  <conditionalFormatting sqref="F38:F607 H38:H607 D2:D607 F24:F37 H2:H37 F11">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -895,8 +1125,176 @@
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F2),E2="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F2),E2="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F3),E3="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F3),E3="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F4),E4="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F4),E4="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F5),E5="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F5),E5="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F6),E6="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F6),E6="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F7),E7="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F7),E7="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F8),E8="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F8),E8="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F9),E9="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F9),E9="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F10),E10="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F10),E10="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F12),E12="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F12),E12="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F13),E13="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F13),E13="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F14),E14="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F14),E14="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F15),E15="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F15),E15="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F16),E16="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F16),E16="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F19),E19="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F19),E19="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F20),E20="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F20),E20="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F17),E17="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F17),E17="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F18),E18="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F18),E18="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F21),E21="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F21),E21="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F22),E22="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F22),E22="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F23),E23="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F23),E23="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C34 E2:E34 G2:G34" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C44 E2:E44 G2:G44" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update Acceptance Test Plan
Test the rest of the stories implemented and added Sprint 3 acceptance
criteria (except for Player Help, because we're waiting on the
instructors).

Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="84">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">Team Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Your team name as "term-swen-261-sec-letter name", e.g. 2171-swen-261-10-a Speedy Racers</t>
+    <t xml:space="preserve">2175-swen-261-13-b Checker Masters</t>
   </si>
   <si>
     <t xml:space="preserve">Testing Team Name</t>
@@ -84,7 +84,8 @@
     <t xml:space="preserve">Given that I am on the Signin page when I enter a name that contains one or more characters that are not alphanumeric or spaces and click the Sign-in button then I expect the system to reject this name and return the Signin form.</t>
   </si>
   <si>
-    <t xml:space="preserve">SJD; 2/28/18; takes non-alphanumerical characters; SJD; 2/28/18</t>
+    <t xml:space="preserve">SJD; 2/28/18; takes non-alphanumerical characters;
+SJD; 2/28/18; Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Given that someone else with my name has signed-in when I enter my name in the sign-in form then I expect the system to reject my sign-in and return the sign-in form for me to try a different name.</t>
@@ -108,6 +109,12 @@
     <t xml:space="preserve">Given that the player I selected is already in a game when I select that player then the system will return me to the Home page with an error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">MTD; 4/4/18; N/A for the future as now you can only click on players if they are not in a game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View from the Home page.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
   </si>
   <si>
@@ -156,7 +163,8 @@
     <t xml:space="preserve">Given that I am in a game and it's my turn, when I make an invalid move, then the move should not complete and I should see an error saying I tried to make an invalid move.</t>
   </si>
   <si>
-    <t xml:space="preserve">MTD; 3/27/18; Moving a piece to a valid location, then moving it to any other location, causes a NullPointerException.</t>
+    <t xml:space="preserve">MTD; 3/27/18; Moving a piece to a valid location, then moving it to any other location, causes a NullPointerException.
+MTD; 4/4/18; Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Jumps</t>
@@ -165,73 +173,112 @@
     <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when there is an opponents piece I can capture then I am able to make a single jump move and take that piece off the board and advance my piece.</t>
   </si>
   <si>
+    <t xml:space="preserve">MTD; 4/4/18; When taking a jump move and undoing it, you can’t make the move anymore (the piece you jumped was removed from the turn’s board)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when there are 2 or more opponents pieces that I can capture then I am able to make a multiple jump move and move those pieces off the board and advance my piece</t>
   </si>
   <si>
+    <t xml:space="preserve">MTD; 4/4/18</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when I have multiple jumps that I can take then I am able to choose which jump I can make</t>
   </si>
   <si>
+    <t xml:space="preserve">Game Over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when I win/lose the game then I expect to redirected back to the Home Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when it is my turn and I am unable to  make a move then I will lose the game and be redirected to the Home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when all my pieces have been eliminated from the board then I will lose the game and be redirected to the Homepage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game, when my opponent loses the game, then I will win the game and be redirected to the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forfeiting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player when I am in a game then I expect to be able to forfeit the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game when I quit the application then I expect to forfeit the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player when I forfeit a game then I expect to be redirected to the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player in a game, when my opponent forfeits the game then I will win the game and be redirected to the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTD; 4/4/18; 500 error given</t>
+  </si>
+  <si>
     <t xml:space="preserve">Forced Moves</t>
   </si>
   <si>
     <t xml:space="preserve">Given that I am a Player in a game when it is my turn and a jump move is possible then I have to make the full jump move in order to advance the game</t>
   </si>
   <si>
+    <t xml:space="preserve">Only test the stories above this one. This story and below are not yet implemented</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given that I am a Player in a game when it is my turn and a multiple jump move is possible then I must complete the entirety of the multiple jump move</t>
   </si>
   <si>
     <t xml:space="preserve">Given that I am in a game, when it is my turn and more than one jump moves are possible, then I am forced to choose one of them to fully jump through.</t>
   </si>
   <si>
-    <t xml:space="preserve">Game Over</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player in a game when I win/lose the game then I expect to redirected back to the Home Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player in a game when it is my turn and I am unable to  make a move then I will lose the game and be redirected to the Home page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player in a game when all my pieces have been eliminated from the board then I will lose the game and be redirected to the Homepage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player in a game, when my opponent loses the game, then I will win the game and be redirected to the home page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forfeiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player when I am in a game then I expect to be able to forfeit the game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player in a game when I quit the application then I expect to forfeit the game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player when I forfeit a game then I expect to be redirected to the home page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given that I am a Player in a game, when my opponent forfeits the game then I will win the game and be redirected to the home page.</t>
-  </si>
-  <si>
     <t xml:space="preserve">King Creation</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am a Player in a game when one of my pieces makes it to the row furthest from me then that piece will become a King piece.</t>
+  </si>
+  <si>
     <t xml:space="preserve">King Movement</t>
   </si>
   <si>
+    <t xml:space="preserve">Given that I am a Player in a game when I have a King piece then it is able to move both forward and backward diagonally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a player in a game when I have a King piece and a multi jump move is possible then that move can be any combination of forward and backward jumps.</t>
+  </si>
+  <si>
     <t xml:space="preserve">King Capturing</t>
   </si>
   <si>
+    <t xml:space="preserve">Given I have a King when I jump a piece then I expect it to be removed properly.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Storing Replays</t>
   </si>
   <si>
+    <t xml:space="preserve">Given I am a Player when I complete a game then I expect my game to be stored as a replay for later viewing.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Listing Replays</t>
   </si>
   <si>
+    <t xml:space="preserve">Given I am a Player when I am on the home page then I expect to see a list of my past games as replays.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Viewing Replays</t>
   </si>
   <si>
-    <t xml:space="preserve">AI Game Request</t>
+    <t xml:space="preserve">Given I am a Player with replays when I see the list of replays then I expect to see a way to view the replay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am a Player with replays when I click to view a reply then I expect to be taken to a replay view of the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given that I am a Player with replays when I view a replay then I am able to view each move in the replay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player Help</t>
   </si>
 </sst>
 </file>
@@ -510,7 +557,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -560,12 +607,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="E21" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topRight" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,11 +620,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="60"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="60"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="46.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="60"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="46.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="60"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="46.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="4" width="10.89"/>
   </cols>
   <sheetData>
@@ -747,7 +794,7 @@
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="46.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
         <v>26</v>
@@ -757,12 +804,18 @@
         <v>14</v>
       </c>
       <c r="E11" s="8"/>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="G11" s="8"/>
+      <c r="H11" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="73.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="3" t="s">
@@ -777,7 +830,7 @@
     <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="3" t="s">
@@ -792,7 +845,7 @@
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="3" t="s">
@@ -807,7 +860,7 @@
     <row r="15" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="3" t="s">
@@ -822,7 +875,7 @@
     <row r="16" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="3" t="s">
@@ -834,14 +887,17 @@
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="8"/>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="3" t="s">
         <v>15</v>
@@ -849,11 +905,14 @@
       <c r="G17" s="8"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" s="8"/>
+      <c r="D18" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="3" t="s">
         <v>15</v>
@@ -861,255 +920,438 @@
       <c r="G18" s="8"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C19" s="8"/>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="8"/>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" s="8"/>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C22" s="8"/>
+      <c r="D22" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" s="8"/>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C24" s="8"/>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E24" s="8"/>
+      <c r="F24" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="G24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C25" s="8"/>
+      <c r="D25" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E25" s="8"/>
+      <c r="F25" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C26" s="8"/>
+      <c r="D26" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E26" s="8"/>
+      <c r="F26" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C27" s="8"/>
+      <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E27" s="8"/>
+      <c r="F27" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="E28" s="8"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C29" s="8"/>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E29" s="8"/>
+      <c r="F29" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C30" s="8"/>
+      <c r="D30" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E30" s="8"/>
+      <c r="F30" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C31" s="8"/>
+      <c r="D31" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E31" s="8"/>
+      <c r="F31" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C32" s="8"/>
+      <c r="D32" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E32" s="8"/>
+      <c r="F32" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C33" s="8"/>
+      <c r="D33" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E33" s="8"/>
+      <c r="F33" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C34" s="8"/>
+      <c r="D34" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E34" s="8"/>
+      <c r="F34" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C35" s="8"/>
+      <c r="D35" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E35" s="8"/>
+      <c r="F35" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G35" s="8"/>
-    </row>
-    <row r="36" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C36" s="8"/>
+      <c r="D36" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E36" s="8"/>
+      <c r="F36" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C37" s="8"/>
+      <c r="D37" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E37" s="8"/>
+      <c r="F37" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C38" s="8"/>
+      <c r="D38" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E38" s="8"/>
+      <c r="F38" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C39" s="8"/>
+      <c r="D39" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E39" s="8"/>
+      <c r="F39" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>64</v>
+    <row r="40" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C40" s="8"/>
       <c r="E40" s="8"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C41" s="8"/>
+      <c r="D41" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E41" s="8"/>
+      <c r="F41" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C42" s="8"/>
+      <c r="D42" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E42" s="8"/>
+      <c r="F42" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>67</v>
+        <v>77</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C43" s="8"/>
+      <c r="D43" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E43" s="8"/>
+      <c r="F43" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C44" s="8"/>
+      <c r="D44" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E44" s="8"/>
+      <c r="F44" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G44" s="8"/>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="8"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C38:C607 E38:E607 G2:G607 C2:C37 E2:E37">
+  <conditionalFormatting sqref="E34:E610 G12:G610 C27:C610 E2:E10 G2:G10 C2:C10 E27:E33 C12:C26 E12:E26">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Pass"</formula>
     </cfRule>
@@ -1117,7 +1359,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:F607 H38:H607 D2:D607 F24:F37 H2:H37 F11">
+  <conditionalFormatting sqref="H12:H610 D27:D610 H2:H10 D2:D10 F24 F41:F610 D12:D26 F27:F38">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -1293,8 +1535,48 @@
       <formula>AND(ISBLANK(F23),E23="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G11 C11 E11">
+    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11 H11 F11">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(D11),C11="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(D11),C11="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F25),E25="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F25),E25="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F26),E26="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F26),E26="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39:F40">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>AND(ISBLANK(F39),E39="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(ISBLANK(F39),E39="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C44 E2:E44 G2:G44" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C47 E2:E47 G2:G47" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update test plan for forfeit bug
Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -215,7 +215,8 @@
     <t xml:space="preserve">Given that I am a Player in a game, when my opponent forfeits the game then I will win the game and be redirected to the home page.</t>
   </si>
   <si>
-    <t xml:space="preserve">MTD; 4/4/18; 500 error given</t>
+    <t xml:space="preserve">MTD; 4/4/18; 500 error given
+MTD; 4/5/18; Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Forced Moves</t>
@@ -609,10 +610,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="E21" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="topRight" activeCell="H35" activeCellId="0" sqref="H35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C22" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topRight" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,7 +1149,7 @@
       </c>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Update test plan as the refactor fixed a bug
Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -173,7 +173,8 @@
     <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when there is an opponents piece I can capture then I am able to make a single jump move and take that piece off the board and advance my piece.</t>
   </si>
   <si>
-    <t xml:space="preserve">MTD; 4/4/18; When taking a jump move and undoing it, you can’t make the move anymore (the piece you jumped was removed from the turn’s board)</t>
+    <t xml:space="preserve">MTD; 4/4/18; When taking a jump move and undoing it, you can’t make the move anymore (the piece you jumped was removed from the turn’s board)
+MTD; 4/5/18; Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Given that I am a Player in a game and it is currently my turn in the game when there are 2 or more opponents pieces that I can capture then I am able to make a multiple jump move and move those pieces off the board and advance my piece</t>
@@ -610,10 +611,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C22" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="topRight" activeCell="F28" activeCellId="0" sqref="F28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C14" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topRight" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1000,7 +1001,7 @@
       </c>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Update Test Plan for Kings
Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="93">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -245,9 +245,6 @@
     <t xml:space="preserve">Given that I am a Player in a game when it is my turn and a jump move is possible then I have to make the full jump move in order to advance the game</t>
   </si>
   <si>
-    <t xml:space="preserve">Only test the stories above this one. This story and below are not yet implemented</t>
-  </si>
-  <si>
     <t xml:space="preserve">Given that I am a Player in a game when it is my turn and a multiple jump move is possible then I must complete the entirety of the multiple jump move</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t xml:space="preserve">Given that I am a Player in a game when one of my pieces makes it to the row furthest from me then that piece will become a King piece.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTD; 4/11/18</t>
   </si>
   <si>
     <t xml:space="preserve">King Movement</t>
@@ -1005,10 +1005,10 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="E31" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topRight" activeCell="H41" activeCellId="0" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1715,7 +1715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1731,13 +1731,10 @@
         <v>30</v>
       </c>
       <c r="G35" s="8"/>
-      <c r="H35" s="3" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="3" t="s">
@@ -1751,7 +1748,7 @@
     </row>
     <row r="37" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="3" t="s">
@@ -1763,12 +1760,12 @@
       </c>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="3" t="s">
@@ -1778,9 +1775,14 @@
       <c r="F38" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>76</v>
       </c>
@@ -1795,17 +1797,27 @@
       <c r="F39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C40" s="8"/>
       <c r="E40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>79</v>
       </c>
@@ -1820,7 +1832,12 @@
       <c r="F41" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="8"/>
+      <c r="G41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">

</xml_diff>

<commit_message>
Update test plan for Storing Replays
Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="93">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -1005,10 +1005,10 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="E31" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="topRight" activeCell="H41" activeCellId="0" sqref="H41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="E34" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topRight" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1839,7 +1839,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>81</v>
       </c>
@@ -1854,7 +1854,12 @@
       <c r="F42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="8"/>
+      <c r="G42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">

</xml_diff>

<commit_message>
Reset player help section of acceptance test plan
Signed-off-by: Mark Drobnak <mtd8050@rit.edu>
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="96">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -314,13 +314,10 @@
     <t xml:space="preserve">Given I am a player when I am in a game then I expect to have  a link to request help.</t>
   </si>
   <si>
-    <t xml:space="preserve">KC; 4/11/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I am a player when I click the request help link then I expect to be redirected to a help page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given I am a player when I am on the help page then I expect to be able to return to my game.</t>
+    <t xml:space="preserve">Given I am a player when I click the request help link then I expect to be shown where I can make a move.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am a player when I make a move after requesting help then I expect the valid move spaces to no longer be indicated.</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1010,10 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="G35" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="topRight" activeCell="H47" activeCellId="0" sqref="H47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="G34" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topRight" activeCell="G49" activeCellId="0" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1956,7 +1953,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
         <v>92</v>
       </c>
@@ -1971,34 +1968,19 @@
       <c r="F47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G47" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="3" t="s">
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="G49" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E10 G2:G10 C2:C10 C12:C610 E12:E610 G12:G610">

</xml_diff>